<commit_message>
Layout e logica atualizados
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Layout</t>
   </si>
@@ -40,13 +40,16 @@
   <si>
     <t>Lógica</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -77,11 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:L17"/>
+  <dimension ref="C2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +451,51 @@
       <c r="F17">
         <v>3</v>
       </c>
+      <c r="H17" s="4">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>41971</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>41972</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>SUM(D17:D19)</f>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E17:E19)</f>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>SUM(F17:F19)</f>
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <f>SUM(D20:F20)</f>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>